<commit_message>
Fixed a bug in the test project
</commit_message>
<xml_diff>
--- a/doc/Sprint+Backlog.xlsx
+++ b/doc/Sprint+Backlog.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="42">
   <si>
     <t>Backlog Item</t>
   </si>
@@ -156,8 +156,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -221,6 +221,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,7 +240,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -256,11 +269,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -272,7 +288,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$42:$E$42</c:f>
+              <c:f>Sprint1!$D$42:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -287,7 +303,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$43:$E$43</c:f>
+              <c:f>Sprint1!$D$43:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -300,6 +316,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -312,7 +329,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$J$2</c:f>
+              <c:f>Sprint1!$E$2:$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -339,7 +356,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$37:$J$37</c:f>
+              <c:f>Sprint1!$E$37:$J$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -364,16 +381,25 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="66898176"/>
-        <c:axId val="63320448"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="86717184"/>
+        <c:axId val="86719104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66898176"/>
+        <c:axId val="86717184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -392,18 +418,22 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63320448"/>
+        <c:crossAx val="86719104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="63320448"/>
+        <c:axId val="86719104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -423,10 +453,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66898176"/>
+        <c:crossAx val="86717184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -434,9 +467,11 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -556,6 +591,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -590,6 +626,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -765,23 +802,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="5.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1"/>
-    <row r="2" spans="1:10">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -797,28 +842,26 @@
       <c r="E2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
         <v>4</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -834,23 +877,23 @@
       <c r="E4" s="4">
         <v>20</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>20</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>14</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>12</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>11</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -863,23 +906,23 @@
       <c r="E5" s="4">
         <v>15</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>15</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5" s="5">
-        <v>2</v>
-      </c>
-      <c r="J5" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -892,23 +935,23 @@
       <c r="E6" s="4">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>10</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="4">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="4">
         <v>9</v>
       </c>
-      <c r="I6" s="5">
-        <v>2</v>
-      </c>
-      <c r="J6" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="I6" s="4">
+        <v>2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -921,23 +964,23 @@
       <c r="E7" s="4">
         <v>3</v>
       </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7" s="5">
-        <v>1</v>
-      </c>
-      <c r="J7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+      <c r="G7" s="4">
+        <v>3</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>1</v>
+      </c>
+      <c r="J7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -950,29 +993,26 @@
       <c r="E8" s="4">
         <v>20</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>20</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="4">
         <v>20</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="4">
         <v>20</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>15</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -988,23 +1028,23 @@
       <c r="E10" s="4">
         <v>5</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>5</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="4">
         <v>5</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>5</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -1017,23 +1057,23 @@
       <c r="E11" s="4">
         <v>3</v>
       </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="F11" s="4">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>1</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1</v>
+      </c>
+      <c r="J11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -1046,23 +1086,23 @@
       <c r="E12" s="4">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -1075,23 +1115,23 @@
       <c r="E13" s="4">
         <v>2</v>
       </c>
-      <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="F13" s="4">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>27</v>
       </c>
@@ -1104,29 +1144,32 @@
       <c r="E14" s="4">
         <v>3</v>
       </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="3" customFormat="1">
+      <c r="F14" s="4">
+        <v>3</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
+      <c r="H14" s="4">
+        <v>3</v>
+      </c>
+      <c r="I14" s="4">
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1142,23 +1185,23 @@
       <c r="E16" s="4">
         <v>3</v>
       </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-      <c r="I16" s="5">
-        <v>2</v>
-      </c>
-      <c r="J16" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="F16" s="4">
+        <v>3</v>
+      </c>
+      <c r="G16" s="4">
+        <v>3</v>
+      </c>
+      <c r="H16" s="4">
+        <v>3</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -1171,23 +1214,23 @@
       <c r="E17" s="4">
         <v>2</v>
       </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17" s="5">
-        <v>2</v>
-      </c>
-      <c r="J17" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2</v>
+      </c>
+      <c r="J17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -1200,29 +1243,26 @@
       <c r="E18" s="4">
         <v>2</v>
       </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-      <c r="I18" s="5">
-        <v>2</v>
-      </c>
-      <c r="J18" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="F18" s="4">
+        <v>2</v>
+      </c>
+      <c r="G18" s="4">
+        <v>2</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2</v>
+      </c>
+      <c r="I18" s="4">
+        <v>2</v>
+      </c>
+      <c r="J18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1238,23 +1278,23 @@
       <c r="E20" s="4">
         <v>1</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20" s="5">
-        <v>1</v>
-      </c>
-      <c r="J20" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="H20" s="4">
+        <v>1</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>15</v>
       </c>
@@ -1267,23 +1307,23 @@
       <c r="E21" s="4">
         <v>3</v>
       </c>
-      <c r="F21">
-        <v>3</v>
-      </c>
-      <c r="G21">
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <v>3</v>
-      </c>
-      <c r="I21" s="5">
-        <v>3</v>
-      </c>
-      <c r="J21" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="F21" s="4">
+        <v>3</v>
+      </c>
+      <c r="G21" s="4">
+        <v>3</v>
+      </c>
+      <c r="H21" s="4">
+        <v>3</v>
+      </c>
+      <c r="I21" s="4">
+        <v>3</v>
+      </c>
+      <c r="J21" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>16</v>
       </c>
@@ -1296,23 +1336,23 @@
       <c r="E22" s="4">
         <v>2</v>
       </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>2</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-      <c r="I22" s="5">
-        <v>2</v>
-      </c>
-      <c r="J22" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="F22" s="4">
+        <v>2</v>
+      </c>
+      <c r="G22" s="4">
+        <v>2</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2</v>
+      </c>
+      <c r="I22" s="4">
+        <v>2</v>
+      </c>
+      <c r="J22" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>17</v>
       </c>
@@ -1325,29 +1365,26 @@
       <c r="E23" s="4">
         <v>2</v>
       </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="I23" s="5">
-        <v>2</v>
-      </c>
-      <c r="J23" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="F23" s="4">
+        <v>2</v>
+      </c>
+      <c r="G23" s="4">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4">
+        <v>2</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2</v>
+      </c>
+      <c r="J23" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1363,23 +1400,23 @@
       <c r="E25" s="4">
         <v>10</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="4">
         <v>10</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="4">
         <v>10</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="4">
         <v>10</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="4">
         <v>10</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>15</v>
       </c>
@@ -1392,23 +1429,23 @@
       <c r="E26" s="4">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="4">
         <v>4</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="4">
         <v>4</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="4">
         <v>4</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="4">
         <v>4</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J26" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -1421,29 +1458,26 @@
       <c r="E27" s="4">
         <v>20</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="4">
         <v>20</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="4">
         <v>5</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
+      <c r="I27" s="4">
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" s="5" customFormat="1">
+    </row>
+    <row r="29" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>30</v>
       </c>
@@ -1459,23 +1493,23 @@
       <c r="E29" s="4">
         <v>2</v>
       </c>
-      <c r="F29" s="5">
-        <v>0</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5">
-        <v>0</v>
-      </c>
-      <c r="I29" s="5">
-        <v>0</v>
-      </c>
-      <c r="J29" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="5" customFormat="1">
+      <c r="F29" s="4">
+        <v>0</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="4">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
@@ -1488,23 +1522,23 @@
       <c r="E30" s="4">
         <v>3</v>
       </c>
-      <c r="F30" s="5">
-        <v>1</v>
-      </c>
-      <c r="G30" s="5">
-        <v>1</v>
-      </c>
-      <c r="H30" s="5">
-        <v>0</v>
-      </c>
-      <c r="I30" s="5">
-        <v>0</v>
-      </c>
-      <c r="J30" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="5" customFormat="1">
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="4">
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>33</v>
       </c>
@@ -1517,23 +1551,23 @@
       <c r="E31" s="4">
         <v>5</v>
       </c>
-      <c r="F31" s="5">
-        <v>0</v>
-      </c>
-      <c r="G31" s="5">
-        <v>0</v>
-      </c>
-      <c r="H31" s="5">
-        <v>0</v>
-      </c>
-      <c r="I31" s="5">
-        <v>0</v>
-      </c>
-      <c r="J31" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="5" customFormat="1">
+      <c r="F31" s="4">
+        <v>0</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="4">
+        <v>0</v>
+      </c>
+      <c r="J31" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>34</v>
       </c>
@@ -1546,23 +1580,23 @@
       <c r="E32" s="4">
         <v>7</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="4">
         <v>7</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <v>7</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="4">
         <v>7</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="4">
         <v>5</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J32" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>35</v>
       </c>
@@ -1575,36 +1609,33 @@
       <c r="E33" s="4">
         <v>7</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="4">
         <v>7</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="4">
         <v>5</v>
       </c>
-      <c r="H33">
-        <v>2</v>
-      </c>
-      <c r="I33" s="5">
-        <v>0</v>
-      </c>
-      <c r="J33" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10">
+      <c r="H33" s="4">
+        <v>2</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-    </row>
-    <row r="35" spans="2:10">
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-    </row>
-    <row r="36" spans="2:10">
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-    </row>
-    <row r="37" spans="2:10">
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="6" t="s">
         <v>38</v>
       </c>
@@ -1616,51 +1647,51 @@
         <f>SUM(E4:E36)</f>
         <v>155</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="4">
         <f>SUM(F4:F36)</f>
         <v>146</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="4">
         <f>SUM(G4:G36)</f>
         <v>106</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="4">
         <f>SUM(H4:H33)</f>
         <v>93</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="4">
         <f>SUM(I4:I33)</f>
         <v>70</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="4">
         <f>SUM(J4:J33)</f>
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="2:10">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C40" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:10">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="8">
         <v>0</v>
       </c>
-      <c r="E42" s="8">
+      <c r="E42" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="2:10">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="8">
         <v>155</v>
       </c>
-      <c r="E43" s="8">
+      <c r="E43" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1678,19 +1709,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" s="5" customFormat="1">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1706,24 +1753,268 @@
       <c r="E2" s="7">
         <v>0</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2">
         <v>4</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
       <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="4">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1737,12 +2028,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>